<commit_message>
maj git action test unitaire
</commit_message>
<xml_diff>
--- a/Test3.xlsx
+++ b/Test3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastienmorichon/OpenClassRooms/DATA SCIENTIST/DS-PROJET-07/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A00EE4-0E32-C14D-AA08-51E07EDC0F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552C8125-CC0D-AD43-A17B-F65E476D35ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{87285369-A446-F441-B6EF-75452CEED644}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="332">
   <si>
     <t>SK_ID_CURR</t>
   </si>
@@ -1013,6 +1013,9 @@
   </si>
   <si>
     <t>-0.07086191470325082</t>
+  </si>
+  <si>
+    <t>TARGET</t>
   </si>
 </sst>
 </file>
@@ -1873,15 +1876,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81240BE2-74EF-AA4B-A228-5E69C2205837}">
-  <dimension ref="A1:IK3"/>
+  <dimension ref="A1:IL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HR1" workbookViewId="0">
-      <selection activeCell="HT11" sqref="HT11"/>
+    <sheetView tabSelected="1" topLeftCell="HV1" workbookViewId="0">
+      <selection activeCell="HV1" sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:245" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:246" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2600,22 +2603,25 @@
         <v>238</v>
       </c>
       <c r="IG1" t="s">
+        <v>331</v>
+      </c>
+      <c r="IH1" t="s">
         <v>239</v>
       </c>
-      <c r="IH1" t="s">
+      <c r="II1" t="s">
         <v>240</v>
       </c>
-      <c r="II1" t="s">
+      <c r="IJ1" t="s">
         <v>241</v>
       </c>
-      <c r="IJ1" t="s">
+      <c r="IK1" t="s">
         <v>242</v>
       </c>
-      <c r="IK1" t="s">
+      <c r="IL1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:245" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:246" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3333,23 +3339,26 @@
       <c r="IF2" t="s">
         <v>248</v>
       </c>
-      <c r="IG2" t="s">
-        <v>248</v>
+      <c r="IG2">
+        <v>1</v>
       </c>
       <c r="IH2" t="s">
+        <v>248</v>
+      </c>
+      <c r="II2" t="s">
         <v>298</v>
       </c>
-      <c r="II2" t="s">
+      <c r="IJ2" t="s">
         <v>299</v>
       </c>
-      <c r="IJ2" t="s">
+      <c r="IK2" t="s">
         <v>300</v>
       </c>
-      <c r="IK2" t="s">
+      <c r="IL2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="3" spans="1:245" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:246" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4064,19 +4073,22 @@
       <c r="IF3" t="s">
         <v>248</v>
       </c>
-      <c r="IG3" t="s">
-        <v>248</v>
+      <c r="IG3">
+        <v>0</v>
       </c>
       <c r="IH3" t="s">
+        <v>248</v>
+      </c>
+      <c r="II3" t="s">
         <v>327</v>
       </c>
-      <c r="II3" t="s">
+      <c r="IJ3" t="s">
         <v>328</v>
       </c>
-      <c r="IJ3" t="s">
+      <c r="IK3" t="s">
         <v>329</v>
       </c>
-      <c r="IK3" t="s">
+      <c r="IL3" t="s">
         <v>330</v>
       </c>
     </row>

</xml_diff>